<commit_message>
Code updates, interface updates, Preferences updates, attempting to rebuild for Android
</commit_message>
<xml_diff>
--- a/Docs/Excel/Excel Date Testing.xlsx
+++ b/Docs/Excel/Excel Date Testing.xlsx
@@ -341,7 +341,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,25 +429,34 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>43171</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.84599999999999997</v>
+      </c>
       <c r="C8" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E8" s="1">
-        <f ca="1">NOW()</f>
-        <v>43171.51140625</v>
-      </c>
+        <v>43171.845999999998</v>
+      </c>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>43171.652524756901</v>
+      </c>
       <c r="C9" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>43171.652524756901</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>43171.676977661999</v>
+      </c>
       <c r="C10" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>43171.676977661999</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>